<commit_message>
updated for web publishing as version 1.
</commit_message>
<xml_diff>
--- a/01_Docs/03_StartingOrder/startingorder_draw.xlsx
+++ b/01_Docs/03_StartingOrder/startingorder_draw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jpngym.sharepoint.com/sites/TRA885/Shared Documents/03_全日本選手権/2023/01_Docs/03_StartingOrder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{EB150D8F-0580-3245-9C03-9BC8C0B20555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC10921-2582-4F4D-8E39-758ABB6CE10D}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{EB150D8F-0580-3245-9C03-9BC8C0B20555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04161B18-8D5E-CF41-8FAE-432F6A774B95}"/>
   <bookViews>
     <workbookView xWindow="34500" yWindow="620" windowWidth="34160" windowHeight="28040" xr2:uid="{50167267-AC88-2040-98A1-F7485C4A059D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>決勝</t>
     <rPh sb="0" eb="2">
@@ -128,6 +128,16 @@
       <t xml:space="preserve">ヨセン </t>
     </rPh>
     <rPh sb="3" eb="5">
+      <t xml:space="preserve">ジュンイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>予選2 順位</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヨセン </t>
+    </rPh>
+    <rPh sb="4" eb="6">
       <t xml:space="preserve">ジュンイ </t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -578,62 +588,62 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,7 +1020,7 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20"/>
@@ -1027,88 +1037,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="19" customFormat="1" ht="26">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" s="19" customFormat="1" ht="23">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
     </row>
     <row r="3" spans="1:12" ht="21" thickBot="1"/>
     <row r="4" spans="1:12" ht="22" thickTop="1" thickBot="1">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12" ht="14" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="6" spans="1:12" ht="21" thickBot="1">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" spans="1:12" ht="8" customHeight="1" thickBot="1"/>
     <row r="8" spans="1:12">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="E8" s="29" t="s">
+      <c r="C8" s="23"/>
+      <c r="E8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="H8" s="27" t="s">
+      <c r="F8" s="25"/>
+      <c r="H8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="28"/>
-      <c r="K8" s="29" t="s">
+      <c r="I8" s="23"/>
+      <c r="K8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="30"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:12" ht="21" thickBot="1">
       <c r="B9" s="9" t="s">
@@ -1127,17 +1137,17 @@
         <v>3</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>3</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="12">
@@ -1169,7 +1179,7 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="21"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1199,7 +1209,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="21"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1229,7 +1239,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="21"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1259,7 +1269,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="21"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1289,7 +1299,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="21"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1319,7 +1329,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="21"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1349,7 +1359,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="21" thickBot="1">
-      <c r="A17" s="21"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1379,7 +1389,7 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="21"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -1401,7 +1411,7 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="21"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -1423,7 +1433,7 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="21"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -1445,7 +1455,7 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" ht="21" thickBot="1">
-      <c r="A21" s="22"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="7">
         <v>12</v>
       </c>
@@ -1467,7 +1477,7 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="12">
@@ -1491,7 +1501,7 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="21"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="5">
         <v>2</v>
       </c>
@@ -1513,7 +1523,7 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="21"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="5">
         <v>3</v>
       </c>
@@ -1535,7 +1545,7 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="21"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="5">
         <v>4</v>
       </c>
@@ -1557,7 +1567,7 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="21"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="5">
         <v>5</v>
       </c>
@@ -1579,7 +1589,7 @@
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="21"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="5">
         <v>6</v>
       </c>
@@ -1601,7 +1611,7 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="21"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="5">
         <v>7</v>
       </c>
@@ -1623,7 +1633,7 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="21"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="5">
         <v>8</v>
       </c>
@@ -1645,7 +1655,7 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="21"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="5">
         <v>9</v>
       </c>
@@ -1667,7 +1677,7 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="21"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="5">
         <v>10</v>
       </c>
@@ -1689,7 +1699,7 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="21"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="5">
         <v>11</v>
       </c>
@@ -1711,7 +1721,7 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" ht="21" thickBot="1">
-      <c r="A33" s="22"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="7">
         <v>12</v>
       </c>
@@ -1747,41 +1757,41 @@
     </row>
     <row r="35" spans="1:12" ht="21" thickBot="1"/>
     <row r="36" spans="1:12" ht="22" thickTop="1" thickBot="1">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
     </row>
     <row r="37" spans="1:12" ht="14" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="38" spans="1:12" ht="21" thickBot="1">
-      <c r="E38" s="34" t="s">
+      <c r="E38" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="36"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="31"/>
     </row>
     <row r="39" spans="1:12" ht="8" customHeight="1" thickBot="1"/>
     <row r="40" spans="1:12">
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="28"/>
-      <c r="H40" s="37" t="s">
+      <c r="F40" s="23"/>
+      <c r="H40" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I40" s="38"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:12">
       <c r="E41" s="3" t="s">
@@ -2040,6 +2050,12 @@
     <sortCondition ref="T18:T25"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="A10:A21"/>
+    <mergeCell ref="A22:A33"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
@@ -2048,12 +2064,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="E38:I38"/>
-    <mergeCell ref="A10:A21"/>
-    <mergeCell ref="A22:A33"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2063,6 +2073,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100940E1E10986D7847BE9C9AC68A86062C" ma:contentTypeVersion="16" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="125f10ebac356ea3a5565510e8d88386">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="952e7e5e-963e-4d92-84b7-491b93135911" xmlns:ns3="1b7a6422-acb0-42a5-b83e-dbe86ecd454b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3322185ac9ec085f88309c373491a520" ns2:_="" ns3:_="">
     <xsd:import namespace="952e7e5e-963e-4d92-84b7-491b93135911"/>
@@ -2305,15 +2324,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2333,6 +2343,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F0567B-BB59-484D-8FE9-9AC5060A3CFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E178238-03E1-49E1-9630-69B9428F0337}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2351,27 +2369,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F0567B-BB59-484D-8FE9-9AC5060A3CFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71B6805B-7C6D-4791-B686-C5643E3CE04C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1b7a6422-acb0-42a5-b83e-dbe86ecd454b"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1b7a6422-acb0-42a5-b83e-dbe86ecd454b"/>
     <ds:schemaRef ds:uri="952e7e5e-963e-4d92-84b7-491b93135911"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>